<commit_message>
2 new suggestions + MC-50247
</commit_message>
<xml_diff>
--- a/Inconsistent namings/Files.xlsx
+++ b/Inconsistent namings/Files.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="713">
   <si>
     <t>Current</t>
   </si>
@@ -2107,6 +2107,57 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Block tag</t>
+  </si>
+  <si>
+    <t>mob_effect/village_hero</t>
+  </si>
+  <si>
+    <t>chiseled_stone_bricks_stone_from_stonecutting</t>
+  </si>
+  <si>
+    <t>*_brick_stonecutting</t>
+  </si>
+  <si>
+    <t>stone_brick_walls_from_stone_stonecutting</t>
+  </si>
+  <si>
+    <t>stone_brick_wall_from_stone_stonecutting</t>
+  </si>
+  <si>
+    <t>chiseled_stone_bricks_from_stone_stonecutting</t>
+  </si>
+  <si>
+    <t>*_bricks_stonecutting</t>
+  </si>
+  <si>
+    <t>Wrong word order</t>
+  </si>
+  <si>
+    <t>Block names never end in "brick" only "bricks"; only the singular items "brick" and "nether_brick" do, but that's not what these are about</t>
+  </si>
+  <si>
+    <t>Block is called "wall", not "walls"</t>
+  </si>
+  <si>
+    <t>Recipe / Recipe advancement</t>
+  </si>
+  <si>
+    <t>mob_effect/hero_of_the_village</t>
+  </si>
+  <si>
+    <t>Following effect ID</t>
+  </si>
+  <si>
+    <t>anvil</t>
+  </si>
+  <si>
+    <t>anvils</t>
+  </si>
+  <si>
+    <t>Plurality, like other block tags</t>
   </si>
 </sst>
 </file>
@@ -2206,7 +2257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2255,6 +2306,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2548,18 +2605,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D353"/>
+  <dimension ref="A1:D358"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B342" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C310" sqref="C310"/>
+      <selection pane="bottomRight" activeCell="D336" sqref="D336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="57.140625" style="5" customWidth="1"/>
     <col min="3" max="3" width="57.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="142.85546875" style="6" customWidth="1"/>
@@ -7014,69 +7071,69 @@
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A319" s="9" t="s">
+      <c r="A319" s="20" t="s">
         <v>70</v>
       </c>
       <c r="B319" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C319" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D319" s="7" t="s">
-        <v>121</v>
+        <v>697</v>
+      </c>
+      <c r="C319" s="14" t="s">
+        <v>708</v>
+      </c>
+      <c r="D319" s="19" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B320" s="7" t="s">
+      <c r="B320" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C320" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D320" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B321" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C320" s="14" t="s">
+      <c r="C321" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D320" s="7" t="s">
+      <c r="D321" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A321" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B321" s="19" t="s">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A322" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B322" s="21" t="s">
         <v>608</v>
       </c>
-      <c r="C321" s="14" t="s">
+      <c r="C322" s="14" t="s">
         <v>609</v>
       </c>
-      <c r="D321" s="7" t="s">
+      <c r="D322" s="7" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A322" s="20"/>
-      <c r="B322" s="19"/>
-      <c r="C322" s="14" t="s">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A323" s="22"/>
+      <c r="B323" s="21"/>
+      <c r="C323" s="14" t="s">
         <v>610</v>
       </c>
-      <c r="D322" s="7" t="s">
+      <c r="D323" s="7" t="s">
         <v>612</v>
-      </c>
-    </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A323" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B323" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="C323" s="7" t="s">
-        <v>613</v>
-      </c>
-      <c r="D323" s="7" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
@@ -7084,10 +7141,10 @@
         <v>70</v>
       </c>
       <c r="B324" s="14" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C324" s="7" t="s">
-        <v>623</v>
+        <v>613</v>
       </c>
       <c r="D324" s="7" t="s">
         <v>628</v>
@@ -7098,10 +7155,10 @@
         <v>70</v>
       </c>
       <c r="B325" s="14" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C325" s="7" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D325" s="7" t="s">
         <v>628</v>
@@ -7112,10 +7169,10 @@
         <v>70</v>
       </c>
       <c r="B326" s="14" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C326" s="7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D326" s="7" t="s">
         <v>628</v>
@@ -7126,13 +7183,13 @@
         <v>70</v>
       </c>
       <c r="B327" s="14" t="s">
-        <v>618</v>
+        <v>625</v>
       </c>
       <c r="C327" s="7" t="s">
-        <v>619</v>
+        <v>627</v>
       </c>
       <c r="D327" s="7" t="s">
-        <v>620</v>
+        <v>628</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -7140,13 +7197,13 @@
         <v>70</v>
       </c>
       <c r="B328" s="14" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="C328" s="7" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="D328" s="7" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
@@ -7154,13 +7211,13 @@
         <v>70</v>
       </c>
       <c r="B329" s="14" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="C329" s="7" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="D329" s="7" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -7168,13 +7225,13 @@
         <v>70</v>
       </c>
       <c r="B330" s="14" t="s">
-        <v>614</v>
+        <v>630</v>
       </c>
       <c r="C330" s="7" t="s">
-        <v>615</v>
+        <v>631</v>
       </c>
       <c r="D330" s="7" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
@@ -7182,13 +7239,13 @@
         <v>70</v>
       </c>
       <c r="B331" s="14" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="C331" s="7" t="s">
-        <v>634</v>
+        <v>615</v>
       </c>
       <c r="D331" s="7" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
@@ -7196,13 +7253,13 @@
         <v>70</v>
       </c>
       <c r="B332" s="14" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C332" s="7" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D332" s="7" t="s">
-        <v>449</v>
+        <v>635</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
@@ -7210,153 +7267,153 @@
         <v>70</v>
       </c>
       <c r="B333" s="14" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C333" s="7" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D333" s="7" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A334" s="4" t="s">
-        <v>640</v>
+      <c r="A334" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="B334" s="14" t="s">
-        <v>649</v>
+        <v>638</v>
       </c>
       <c r="C334" s="7" t="s">
-        <v>650</v>
+        <v>639</v>
       </c>
       <c r="D334" s="7" t="s">
-        <v>651</v>
+        <v>449</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="B335" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="C335" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="D335" s="19" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A336" s="10" t="s">
+        <v>707</v>
+      </c>
+      <c r="B336" s="14" t="s">
+        <v>698</v>
+      </c>
+      <c r="C336" s="14" t="s">
+        <v>702</v>
+      </c>
+      <c r="D336" s="19" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A337" s="10" t="s">
+        <v>707</v>
+      </c>
+      <c r="B337" s="14" t="s">
+        <v>699</v>
+      </c>
+      <c r="C337" s="19" t="s">
+        <v>703</v>
+      </c>
+      <c r="D337" s="19" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A338" s="10" t="s">
+        <v>707</v>
+      </c>
+      <c r="B338" s="14" t="s">
+        <v>700</v>
+      </c>
+      <c r="C338" s="14" t="s">
+        <v>701</v>
+      </c>
+      <c r="D338" s="19" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="B335" s="14" t="s">
+      <c r="B339" s="14" t="s">
+        <v>649</v>
+      </c>
+      <c r="C339" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="D339" s="7" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="B340" s="14" t="s">
         <v>641</v>
       </c>
-      <c r="C335" s="7" t="s">
+      <c r="C340" s="7" t="s">
         <v>642</v>
       </c>
-      <c r="D335" s="7" t="s">
+      <c r="D340" s="7" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A336" s="4" t="s">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="B336" s="14" t="s">
+      <c r="B341" s="14" t="s">
         <v>644</v>
       </c>
-      <c r="C336" s="7" t="s">
+      <c r="C341" s="7" t="s">
         <v>645</v>
       </c>
-      <c r="D336" s="7" t="s">
+      <c r="D341" s="7" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A337" s="4" t="s">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="B337" s="14" t="s">
+      <c r="B342" s="14" t="s">
         <v>646</v>
       </c>
-      <c r="C337" s="7" t="s">
+      <c r="C342" s="7" t="s">
         <v>647</v>
       </c>
-      <c r="D337" s="7" t="s">
+      <c r="D342" s="7" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A338" s="9" t="s">
-        <v>652</v>
-      </c>
-      <c r="B338" s="14" t="s">
-        <v>654</v>
-      </c>
-      <c r="C338" s="7" t="s">
-        <v>668</v>
-      </c>
-      <c r="D338" s="7" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A339" s="9" t="s">
-        <v>652</v>
-      </c>
-      <c r="B339" s="14" t="s">
-        <v>655</v>
-      </c>
-      <c r="C339" s="7" t="s">
-        <v>669</v>
-      </c>
-      <c r="D339" s="7" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A340" s="9" t="s">
-        <v>652</v>
-      </c>
-      <c r="B340" s="14" t="s">
-        <v>656</v>
-      </c>
-      <c r="C340" s="7" t="s">
-        <v>670</v>
-      </c>
-      <c r="D340" s="7" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A341" s="9" t="s">
-        <v>652</v>
-      </c>
-      <c r="B341" s="14" t="s">
-        <v>657</v>
-      </c>
-      <c r="C341" s="7" t="s">
-        <v>671</v>
-      </c>
-      <c r="D341" s="7" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A342" s="9" t="s">
-        <v>652</v>
-      </c>
-      <c r="B342" s="14" t="s">
-        <v>658</v>
-      </c>
-      <c r="C342" s="7" t="s">
-        <v>672</v>
-      </c>
-      <c r="D342" s="7" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="343" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" s="9" t="s">
         <v>652</v>
       </c>
       <c r="B343" s="14" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="C343" s="7" t="s">
-        <v>682</v>
-      </c>
-      <c r="D343" s="16" t="s">
-        <v>683</v>
+        <v>668</v>
+      </c>
+      <c r="D343" s="7" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -7364,10 +7421,10 @@
         <v>652</v>
       </c>
       <c r="B344" s="14" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="C344" s="7" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D344" s="7" t="s">
         <v>653</v>
@@ -7378,10 +7435,10 @@
         <v>652</v>
       </c>
       <c r="B345" s="14" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="C345" s="7" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D345" s="7" t="s">
         <v>653</v>
@@ -7392,10 +7449,10 @@
         <v>652</v>
       </c>
       <c r="B346" s="14" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="C346" s="7" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="D346" s="7" t="s">
         <v>681</v>
@@ -7406,27 +7463,27 @@
         <v>652</v>
       </c>
       <c r="B347" s="14" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="C347" s="7" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="D347" s="7" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="9" t="s">
         <v>652</v>
       </c>
       <c r="B348" s="14" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="C348" s="7" t="s">
-        <v>676</v>
-      </c>
-      <c r="D348" s="7" t="s">
-        <v>681</v>
+        <v>682</v>
+      </c>
+      <c r="D348" s="16" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -7434,10 +7491,10 @@
         <v>652</v>
       </c>
       <c r="B349" s="14" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="C349" s="7" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="D349" s="7" t="s">
         <v>653</v>
@@ -7448,10 +7505,10 @@
         <v>652</v>
       </c>
       <c r="B350" s="14" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="C350" s="7" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="D350" s="7" t="s">
         <v>653</v>
@@ -7462,47 +7519,117 @@
         <v>652</v>
       </c>
       <c r="B351" s="14" t="s">
+        <v>662</v>
+      </c>
+      <c r="C351" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="D351" s="7" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A352" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="B352" s="14" t="s">
+        <v>663</v>
+      </c>
+      <c r="C352" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="D352" s="7" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A353" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="B353" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="C353" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="D353" s="7" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A354" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="B354" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="C354" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="D354" s="7" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A355" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="B355" s="14" t="s">
+        <v>666</v>
+      </c>
+      <c r="C355" s="7" t="s">
+        <v>679</v>
+      </c>
+      <c r="D355" s="7" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A356" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="B356" s="14" t="s">
         <v>667</v>
       </c>
-      <c r="C351" s="7" t="s">
+      <c r="C356" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="D351" s="7" t="s">
+      <c r="D356" s="7" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="352" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A352" s="8" t="s">
+    <row r="357" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A357" s="8" t="s">
         <v>684</v>
       </c>
-      <c r="B352" s="14" t="s">
+      <c r="B357" s="14" t="s">
         <v>685</v>
       </c>
-      <c r="C352" s="7" t="s">
+      <c r="C357" s="7" t="s">
         <v>686</v>
       </c>
-      <c r="D352" s="7" t="s">
+      <c r="D357" s="7" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="353" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A353" s="10" t="s">
+    <row r="358" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A358" s="10" t="s">
         <v>688</v>
       </c>
-      <c r="B353" s="14" t="s">
+      <c r="B358" s="14" t="s">
         <v>689</v>
       </c>
-      <c r="C353" s="7" t="s">
+      <c r="C358" s="7" t="s">
         <v>690</v>
       </c>
-      <c r="D353" s="7" t="s">
+      <c r="D358" s="7" t="s">
         <v>691</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B321:B322"/>
-    <mergeCell ref="A321:A322"/>
+    <mergeCell ref="B322:B323"/>
+    <mergeCell ref="A322:A323"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>